<commit_message>
Created MNIST_CNN_V03. Changed DCT to 2D DTC in V03. Changed Network architecture to adapt to different input sizes. Added Spawner to utilize mutliple GPU.
</commit_message>
<xml_diff>
--- a/Juni/Mappe1.xlsx
+++ b/Juni/Mappe1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz\Documents\0.0 ETH\Bachelorarbeit\27.06._MNIST_CNN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz\Documents\0.0 ETH\Bachelorarbeit\Git\Juni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA721649-1461-4E6F-B423-E5FB0C127170}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12A0A2D-E3D6-40D6-A35E-BAA20ACC13E3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{0EBB454D-EA3D-4894-84B7-1E36106A9039}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>20 epochs per point, 4 full cycles per point, averaged</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>14x14</t>
+  </si>
+  <si>
+    <t>1D DCT</t>
+  </si>
+  <si>
+    <t>Downscaled</t>
+  </si>
+  <si>
+    <t>2D DCT</t>
   </si>
 </sst>
 </file>
@@ -258,7 +267,195 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EFB2-4879-9410-5E9EF2BF1470}"/>
+              <c16:uniqueId val="{00000000-FD7D-4798-A752-D3A3C32CD09C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$4:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>169</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$4:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.97965999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96077495000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FD7D-4798-A752-D3A3C32CD09C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$4:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>169</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$4:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="2">
+                  <c:v>0.96906599999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96600000600000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FD7D-4798-A752-D3A3C32CD09C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -270,11 +467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1268598335"/>
-        <c:axId val="1316256255"/>
+        <c:axId val="1518179888"/>
+        <c:axId val="1522125600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1268598335"/>
+        <c:axId val="1518179888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -331,12 +528,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1316256255"/>
+        <c:crossAx val="1522125600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1316256255"/>
+        <c:axId val="1522125600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,7 +590,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1268598335"/>
+        <c:crossAx val="1518179888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -405,8 +602,46 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1002,23 +1237,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>255270</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>78105</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>78105</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>315829</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>170447</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Diagramm 7">
+        <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EE5FF36-78A7-4584-93CF-C0C82C2AF6B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4831EA3D-8DA6-478E-96D6-04C09AA44A86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1338,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD135B44-2A39-49B0-8146-D824BD037953}">
   <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1352,6 +1587,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
         <v>784</v>
@@ -1384,6 +1630,9 @@
       <c r="C6">
         <v>0.96302500359999998</v>
       </c>
+      <c r="E6">
+        <v>0.96906599999999998</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
@@ -1456,6 +1705,9 @@
       </c>
       <c r="D14">
         <v>0.96077495000000002</v>
+      </c>
+      <c r="E14">
+        <v>0.96600000600000002</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Added Shearlet Compression and a tensor flow based batch downscaling procedure to utilize gpu
</commit_message>
<xml_diff>
--- a/Juni/Mappe1.xlsx
+++ b/Juni/Mappe1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz\Documents\0.0 ETH\Bachelorarbeit\Git\Juni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12A0A2D-E3D6-40D6-A35E-BAA20ACC13E3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B831DE-3030-44D6-9E8C-B93B52B0D82F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{0EBB454D-EA3D-4894-84B7-1E36106A9039}"/>
   </bookViews>
@@ -176,10 +176,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$B$15</c:f>
+              <c:f>Tabelle1!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>784</c:v>
                 </c:pt>
@@ -208,23 +208,32 @@
                   <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>225</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>196</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$4:$C$15</c:f>
+              <c:f>Tabelle1!$C$4:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0.96809997999999997</c:v>
                 </c:pt>
@@ -252,13 +261,13 @@
                 <c:pt idx="8">
                   <c:v>0.96014998799999995</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.95537499999999997</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.95547500249999995</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.95280000499999995</c:v>
                 </c:pt>
               </c:numCache>
@@ -267,7 +276,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FD7D-4798-A752-D3A3C32CD09C}"/>
+              <c16:uniqueId val="{00000000-063F-4895-9ABE-808BF7E8C462}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -300,10 +309,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$B$15</c:f>
+              <c:f>Tabelle1!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>784</c:v>
                 </c:pt>
@@ -332,27 +341,36 @@
                   <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>225</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>196</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$4:$D$15</c:f>
+              <c:f>Tabelle1!$D$4:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0.97965999999999998</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.96077495000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -361,7 +379,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FD7D-4798-A752-D3A3C32CD09C}"/>
+              <c16:uniqueId val="{00000001-063F-4895-9ABE-808BF7E8C462}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -394,10 +412,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$B$15</c:f>
+              <c:f>Tabelle1!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>784</c:v>
                 </c:pt>
@@ -426,28 +444,61 @@
                   <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>225</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>196</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$E$4:$E$15</c:f>
+              <c:f>Tabelle1!$E$4:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.96839989999999998</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>0.96906599999999998</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96912500000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96892498999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96782000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97040000500000001</c:v>
+                </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.96600000600000002</c:v>
+                  <c:v>0.96720001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9674500077</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.96427498</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.96517500280000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -455,7 +506,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FD7D-4798-A752-D3A3C32CD09C}"/>
+              <c16:uniqueId val="{00000002-063F-4895-9ABE-808BF7E8C462}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -467,11 +518,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1518179888"/>
-        <c:axId val="1522125600"/>
+        <c:axId val="108830399"/>
+        <c:axId val="106762575"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1518179888"/>
+        <c:axId val="108830399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,12 +579,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1522125600"/>
+        <c:crossAx val="106762575"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1522125600"/>
+        <c:axId val="106762575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -590,7 +641,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1518179888"/>
+        <c:crossAx val="108830399"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1237,23 +1288,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>623955</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>166203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>315829</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>170447</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>220869</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>176695</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1">
+        <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4831EA3D-8DA6-478E-96D6-04C09AA44A86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{994E3167-BC17-4499-ABAA-3C4C48D4BC93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD135B44-2A39-49B0-8146-D824BD037953}">
-  <dimension ref="B2:H15"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="69" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1608,6 +1659,9 @@
       <c r="D4">
         <v>0.97965999999999998</v>
       </c>
+      <c r="E4">
+        <v>0.96839989999999998</v>
+      </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
@@ -1663,6 +1717,9 @@
       <c r="C9">
         <v>0.95475001000000004</v>
       </c>
+      <c r="E9">
+        <v>0.96912500000000001</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
@@ -1679,6 +1736,9 @@
       <c r="C11">
         <v>0.96207499500000004</v>
       </c>
+      <c r="E11">
+        <v>0.96892498999999999</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
@@ -1687,35 +1747,65 @@
       <c r="C12">
         <v>0.96014998799999995</v>
       </c>
+      <c r="E12">
+        <v>0.96782000000000001</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
-        <v>225</v>
-      </c>
-      <c r="C13">
-        <v>0.95537499999999997</v>
+        <v>256</v>
+      </c>
+      <c r="E13">
+        <v>0.97040000500000001</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="C14">
-        <v>0.95547500249999995</v>
-      </c>
-      <c r="D14">
-        <v>0.96077495000000002</v>
+        <v>0.95537499999999997</v>
       </c>
       <c r="E14">
-        <v>0.96600000600000002</v>
+        <v>0.96720001</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
+        <v>196</v>
+      </c>
+      <c r="C15">
+        <v>0.95547500249999995</v>
+      </c>
+      <c r="D15">
+        <v>0.96077495000000002</v>
+      </c>
+      <c r="E15">
+        <v>0.9674500077</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16">
         <v>169</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>0.95280000499999995</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17">
+        <v>121</v>
+      </c>
+      <c r="E17">
+        <v>0.96427498</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="E18">
+        <v>0.96517500280000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started Working on Cifar10. Created a Dataset input pipeline for Cifar10. Implemented tensorboard integration for Cifar10. Attempted to implement random hyperparameter search, not successfull because dataset iterator does not reset.
</commit_message>
<xml_diff>
--- a/Juni/Mappe1.xlsx
+++ b/Juni/Mappe1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz\Documents\0.0 ETH\Bachelorarbeit\Git\Juni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B831DE-3030-44D6-9E8C-B93B52B0D82F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E7C653-FCDD-47A6-BD21-62EFC00EB121}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{0EBB454D-EA3D-4894-84B7-1E36106A9039}"/>
   </bookViews>
@@ -36,13 +36,13 @@
     <t>14x14</t>
   </si>
   <si>
-    <t>1D DCT</t>
-  </si>
-  <si>
     <t>Downscaled</t>
   </si>
   <si>
     <t>2D DCT</t>
+  </si>
+  <si>
+    <t>Wavelet</t>
   </si>
 </sst>
 </file>
@@ -176,99 +176,57 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$B$18</c:f>
+              <c:f>Tabelle1!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>784</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>729</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>676</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>576</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>529</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>484</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>400</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>361</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>289</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>100</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$4:$C$18</c:f>
+              <c:f>Tabelle1!$C$4:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.96809997999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.96712500000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.96302500359999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.955125004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.95410001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.95475001000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.961499989</c:v>
+                  <c:v>0.97965999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96207499500000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.96014998799999995</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.95537499999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.95547500249999995</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.95280000499999995</c:v>
+                  <c:v>0.96077495000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -276,7 +234,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-063F-4895-9ABE-808BF7E8C462}"/>
+              <c16:uniqueId val="{00000000-9663-4FFA-9145-1A64014E544A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -309,69 +267,84 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$B$18</c:f>
+              <c:f>Tabelle1!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>784</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>729</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>676</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>576</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>529</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>484</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>400</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>361</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>289</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>100</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$4:$D$18</c:f>
+              <c:f>Tabelle1!$D$4:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.97965999999999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.96077495000000002</c:v>
+                  <c:v>0.95483334799999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95856666000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95423329999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95933299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95596665000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9559666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95020000100000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.95156666999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95430000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94603331879999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.923933</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -379,7 +352,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-063F-4895-9ABE-808BF7E8C462}"/>
+              <c16:uniqueId val="{00000001-9663-4FFA-9145-1A64014E544A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -412,92 +385,68 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$B$18</c:f>
+              <c:f>Tabelle1!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>784</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>729</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>676</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>576</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>529</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>484</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>400</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>361</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>289</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>256</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>100</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$E$4:$E$18</c:f>
+              <c:f>Tabelle1!$E$4:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.96839989999999998</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
                   <c:v>0.96906599999999998</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="3">
                   <c:v>0.96912500000000001</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97040000500000001</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96892498999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.96782000000000001</c:v>
+                  <c:v>0.9674500077</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97040000500000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.96720001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.9674500077</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.96427498</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>0.96517500280000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -506,7 +455,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-063F-4895-9ABE-808BF7E8C462}"/>
+              <c16:uniqueId val="{00000002-9663-4FFA-9145-1A64014E544A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -518,11 +467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108830399"/>
-        <c:axId val="106762575"/>
+        <c:axId val="746161823"/>
+        <c:axId val="786343743"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108830399"/>
+        <c:axId val="746161823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,12 +528,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106762575"/>
+        <c:crossAx val="786343743"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106762575"/>
+        <c:axId val="786343743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +590,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108830399"/>
+        <c:crossAx val="746161823"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1289,22 +1238,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>623955</xdr:colOff>
+      <xdr:colOff>623956</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>166203</xdr:rowOff>
+      <xdr:rowOff>166204</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>220869</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>176695</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>701261</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>176144</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
+        <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{994E3167-BC17-4499-ABAA-3C4C48D4BC93}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F87336EC-2A8C-4502-B8CB-893AFD53F8C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1622,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD135B44-2A39-49B0-8146-D824BD037953}">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="69" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E18"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1643,10 +1592,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -1654,10 +1603,10 @@
         <v>784</v>
       </c>
       <c r="C4">
-        <v>0.96809997999999997</v>
+        <v>0.97965999999999998</v>
       </c>
       <c r="D4">
-        <v>0.97965999999999998</v>
+        <v>0.95483334799999997</v>
       </c>
       <c r="E4">
         <v>0.96839989999999998</v>
@@ -1671,29 +1620,32 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
-        <v>729</v>
-      </c>
-      <c r="C5">
-        <v>0.96712500000000001</v>
+        <v>676</v>
+      </c>
+      <c r="D5">
+        <v>0.95856666000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.96906599999999998</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
-        <v>676</v>
-      </c>
-      <c r="C6">
-        <v>0.96302500359999998</v>
-      </c>
-      <c r="E6">
-        <v>0.96906599999999998</v>
+        <v>576</v>
+      </c>
+      <c r="D6">
+        <v>0.95423329999999995</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
-        <v>576</v>
-      </c>
-      <c r="C7">
-        <v>0.955125004</v>
+        <v>484</v>
+      </c>
+      <c r="D7">
+        <v>0.95933299999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.96912500000000001</v>
       </c>
       <c r="G7" t="s">
         <v>2</v>
@@ -1704,108 +1656,70 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
-        <v>529</v>
-      </c>
-      <c r="C8">
-        <v>0.95410001</v>
+        <v>400</v>
+      </c>
+      <c r="D8">
+        <v>0.95596665000000003</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
-        <v>484</v>
-      </c>
-      <c r="C9">
-        <v>0.95475001000000004</v>
-      </c>
-      <c r="E9">
-        <v>0.96912500000000001</v>
+        <v>324</v>
+      </c>
+      <c r="D9">
+        <v>0.9559666</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
-        <v>400</v>
-      </c>
-      <c r="C10">
-        <v>0.961499989</v>
+        <v>256</v>
+      </c>
+      <c r="D10">
+        <v>0.95020000100000002</v>
+      </c>
+      <c r="E10">
+        <v>0.97040000500000001</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
-        <v>361</v>
+        <v>196</v>
       </c>
       <c r="C11">
-        <v>0.96207499500000004</v>
+        <v>0.96077495000000002</v>
+      </c>
+      <c r="D11">
+        <v>0.95156666999999995</v>
       </c>
       <c r="E11">
-        <v>0.96892498999999999</v>
+        <v>0.9674500077</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
-        <v>289</v>
-      </c>
-      <c r="C12">
-        <v>0.96014998799999995</v>
-      </c>
-      <c r="E12">
-        <v>0.96782000000000001</v>
+        <v>144</v>
+      </c>
+      <c r="D12">
+        <v>0.95430000000000004</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
-        <v>256</v>
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>0.94603331879999997</v>
       </c>
       <c r="E13">
-        <v>0.97040000500000001</v>
+        <v>0.96517500280000001</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
-        <v>225</v>
-      </c>
-      <c r="C14">
-        <v>0.95537499999999997</v>
-      </c>
-      <c r="E14">
-        <v>0.96720001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15">
-        <v>196</v>
-      </c>
-      <c r="C15">
-        <v>0.95547500249999995</v>
-      </c>
-      <c r="D15">
-        <v>0.96077495000000002</v>
-      </c>
-      <c r="E15">
-        <v>0.9674500077</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16">
-        <v>169</v>
-      </c>
-      <c r="C16">
-        <v>0.95280000499999995</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17">
-        <v>121</v>
-      </c>
-      <c r="E17">
-        <v>0.96427498</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18">
-        <v>100</v>
-      </c>
-      <c r="E18">
-        <v>0.96517500280000001</v>
+        <v>64</v>
+      </c>
+      <c r="D14">
+        <v>0.923933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>